<commit_message>
calibrated fc current sensor and programed in some safe guards to prevent me from doing stupid things
</commit_message>
<xml_diff>
--- a/Hardware/FCC Power Board/Parts List.xlsx
+++ b/Hardware/FCC Power Board/Parts List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Capacitors</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>3.3 uF</t>
+  </si>
+  <si>
+    <t>E36SR12004</t>
+  </si>
+  <si>
+    <t>SMAJ16CA</t>
+  </si>
+  <si>
+    <t>STPS5L60</t>
+  </si>
+  <si>
+    <t>SMBJ60CA</t>
+  </si>
+  <si>
+    <t>MBR360GOS</t>
   </si>
 </sst>
 </file>
@@ -384,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,6 +443,9 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -468,44 +486,87 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>500</v>
       </c>
-      <c r="C26">
+      <c r="C30">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>2300</v>
       </c>
-      <c r="C27">
+      <c r="C31">
         <v>1</v>
       </c>
     </row>

</xml_diff>